<commit_message>
Atualização Conferência LN - CAR
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_CAR.xlsx
+++ b/Documentação/Planilhas/Conferencia_CAR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="93" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="308">
   <si>
     <t>1</t>
   </si>
@@ -545,9 +545,6 @@
 7-Não aplicável
 8-Pagto Cheque
 9-Pagto Cancelado</t>
-  </si>
-  <si>
-    <t>tfacr2520m000</t>
   </si>
   <si>
     <t>Pegar a primeira e segunda informação da coluna Documento</t>
@@ -984,6 +981,33 @@
   </si>
   <si>
     <t>selecionar o documento desejado e no menu Specific, selecionar "Documentos Relacionados ao Recebimento por Entrada Aberta". Pegar a terceira informação da coluna Nº Doc Recebimento</t>
+  </si>
+  <si>
+    <t>tfacr2523m000</t>
+  </si>
+  <si>
+    <t>Sessão tfacr2523m000</t>
+  </si>
+  <si>
+    <t>Informar na primeira e segunda informação da coluna Nº Doc Recebimento os dados de CD_TRANSACAO_DOCUMENTO e NR_MOVIMENTO. Ir com a seta de navegação "Next Group"  para encontrar o Título de Referência [veremos a indicação do título de origem e também a informação do título de Referência]</t>
+  </si>
+  <si>
+    <t>selecionar o documento desejado e no menu Specific, selecionar "Documentos Relacionados ao Recebimento por Entrada Aberta". Pegar a informação da coluna Data de Recebto.</t>
+  </si>
+  <si>
+    <t>Usar a seguinte regra para pegar a data:</t>
+  </si>
+  <si>
+    <t>Utilizar sempre CD_TRANSACAO_TITULO, NR_TITULO e NR_PROGRAMACAO
+Se Saldo = Saldo Previsto, então pegar a maior data da coluna Data do Recebto.
+Se Saldo = Valor, pegar a Data do Recebto
+Caso contrário, pegar a menor data da coluna Data de Recebto.</t>
+  </si>
+  <si>
+    <t>tfacr2520m000, tfcmg0511m000, tfcmg0510m000 e tfacr2523m000</t>
+  </si>
+  <si>
+    <t>tfacr2520m000</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1061,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1059,6 +1083,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1314,7 +1344,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1368,17 +1398,17 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1392,16 +1422,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1434,6 +1458,12 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1445,6 +1475,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1463,18 +1514,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1807,31 +1846,31 @@
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C7" s="9"/>
     </row>
@@ -1856,7 +1895,7 @@
   <dimension ref="A2:AG22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -2282,17 +2321,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
     <mergeCell ref="I19:I22"/>
     <mergeCell ref="D19:D22"/>
     <mergeCell ref="E19:E22"/>
     <mergeCell ref="F19:F22"/>
     <mergeCell ref="G19:G22"/>
     <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2306,8 +2345,8 @@
   </sheetPr>
   <dimension ref="A2:Q25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -2346,7 +2385,9 @@
         <v>15</v>
       </c>
       <c r="B3" s="30"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
@@ -2418,71 +2459,71 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="26" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="26" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="26" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2796,9 +2837,7 @@
   </sheetPr>
   <dimension ref="A2:AE29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:E26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
@@ -2850,18 +2889,18 @@
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="21">
-      <c r="A4" s="44" t="s">
-        <v>185</v>
-      </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="A4" s="42" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="1"/>
       <c r="P4" s="19"/>
       <c r="AB4" s="2"/>
@@ -3028,7 +3067,7 @@
       <c r="V8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="W8" s="25" t="s">
+      <c r="W8" s="23" t="s">
         <v>9</v>
       </c>
       <c r="X8" s="16" t="s">
@@ -3123,7 +3162,7 @@
       <c r="V9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="W9" s="25" t="s">
+      <c r="W9" s="23" t="s">
         <v>9</v>
       </c>
       <c r="X9" s="16" t="s">
@@ -3162,37 +3201,37 @@
         <v>1</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>130</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L10" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="M10" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="N10" s="16" t="s">
         <v>201</v>
-      </c>
-      <c r="N10" s="16" t="s">
-        <v>202</v>
       </c>
       <c r="O10" s="16" t="s">
         <v>126</v>
@@ -3210,7 +3249,7 @@
         <v>83</v>
       </c>
       <c r="T10" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U10" s="16" t="s">
         <v>84</v>
@@ -3218,7 +3257,7 @@
       <c r="V10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="W10" s="25" t="s">
+      <c r="W10" s="23" t="s">
         <v>9</v>
       </c>
       <c r="X10" s="16" t="s">
@@ -3228,7 +3267,7 @@
         <v>83</v>
       </c>
       <c r="Z10" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AA10" s="16" t="s">
         <v>9</v>
@@ -3257,37 +3296,37 @@
         <v>1</v>
       </c>
       <c r="D11" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>130</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M11" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="N11" s="16" t="s">
         <v>201</v>
-      </c>
-      <c r="N11" s="16" t="s">
-        <v>202</v>
       </c>
       <c r="O11" s="16" t="s">
         <v>126</v>
@@ -3305,7 +3344,7 @@
         <v>83</v>
       </c>
       <c r="T11" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U11" s="16" t="s">
         <v>84</v>
@@ -3313,7 +3352,7 @@
       <c r="V11" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="W11" s="25" t="s">
+      <c r="W11" s="23" t="s">
         <v>9</v>
       </c>
       <c r="X11" s="16" t="s">
@@ -3323,7 +3362,7 @@
         <v>83</v>
       </c>
       <c r="Z11" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AA11" s="16" t="s">
         <v>9</v>
@@ -3352,37 +3391,37 @@
         <v>1</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>130</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L12" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="N12" s="16" t="s">
         <v>212</v>
-      </c>
-      <c r="M12" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="N12" s="16" t="s">
-        <v>213</v>
       </c>
       <c r="O12" s="16" t="s">
         <v>126</v>
@@ -3400,7 +3439,7 @@
         <v>83</v>
       </c>
       <c r="T12" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="U12" s="16" t="s">
         <v>84</v>
@@ -3408,7 +3447,7 @@
       <c r="V12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="W12" s="25" t="s">
+      <c r="W12" s="23" t="s">
         <v>9</v>
       </c>
       <c r="X12" s="16" t="s">
@@ -3418,7 +3457,7 @@
         <v>83</v>
       </c>
       <c r="Z12" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AA12" s="16" t="s">
         <v>9</v>
@@ -3446,88 +3485,88 @@
       <c r="C13" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>214</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>215</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="H13" s="25" t="s">
-        <v>216</v>
+      <c r="H13" s="23" t="s">
+        <v>215</v>
       </c>
       <c r="I13" s="12" t="s">
         <v>1</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K13" s="12" t="s">
         <v>0</v>
       </c>
       <c r="L13" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="M13" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="N13" s="23" t="s">
         <v>218</v>
       </c>
-      <c r="M13" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="N13" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="O13" s="25" t="s">
+      <c r="O13" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="P13" s="25" t="s">
+      <c r="P13" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="Q13" s="25" t="s">
+      <c r="Q13" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="R13" s="25" t="s">
+      <c r="R13" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="S13" s="25" t="s">
+      <c r="S13" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="T13" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="U13" s="25" t="s">
+      <c r="T13" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="U13" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="V13" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="W13" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="X13" s="25" t="s">
+      <c r="V13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="W13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="X13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="Y13" s="25" t="s">
+      <c r="Y13" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="Z13" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="AA13" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB13" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC13" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD13" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE13" s="25" t="s">
+      <c r="Z13" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="AA13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE13" s="23" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3542,37 +3581,37 @@
         <v>1</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>130</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M14" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="N14" s="16" t="s">
         <v>201</v>
-      </c>
-      <c r="N14" s="16" t="s">
-        <v>202</v>
       </c>
       <c r="O14" s="16" t="s">
         <v>126</v>
@@ -3590,7 +3629,7 @@
         <v>83</v>
       </c>
       <c r="T14" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U14" s="16" t="s">
         <v>84</v>
@@ -3598,7 +3637,7 @@
       <c r="V14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="W14" s="25" t="s">
+      <c r="W14" s="23" t="s">
         <v>9</v>
       </c>
       <c r="X14" s="16" t="s">
@@ -3608,7 +3647,7 @@
         <v>83</v>
       </c>
       <c r="Z14" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AA14" s="16" t="s">
         <v>9</v>
@@ -3637,7 +3676,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E15" s="16" t="s">
         <v>9</v>
@@ -3655,19 +3694,19 @@
         <v>1</v>
       </c>
       <c r="J15" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="M15" s="16" t="s">
+      <c r="N15" s="16" t="s">
         <v>240</v>
-      </c>
-      <c r="N15" s="16" t="s">
-        <v>241</v>
       </c>
       <c r="O15" s="16" t="s">
         <v>136</v>
@@ -3685,7 +3724,7 @@
         <v>83</v>
       </c>
       <c r="T15" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U15" s="16" t="s">
         <v>84</v>
@@ -3693,7 +3732,7 @@
       <c r="V15" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="W15" s="25" t="s">
+      <c r="W15" s="23" t="s">
         <v>132</v>
       </c>
       <c r="X15" s="16" t="s">
@@ -3703,7 +3742,7 @@
         <v>83</v>
       </c>
       <c r="Z15" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AA15" s="16" t="s">
         <v>9</v>
@@ -3732,43 +3771,43 @@
         <v>1</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="16" t="s">
         <v>246</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>247</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M16" s="16" t="s">
         <v>150</v>
       </c>
       <c r="N16" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="O16" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="O16" s="16" t="s">
-        <v>251</v>
-      </c>
       <c r="P16" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Q16" s="16" t="s">
         <v>83</v>
@@ -3780,7 +3819,7 @@
         <v>83</v>
       </c>
       <c r="T16" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="U16" s="16" t="s">
         <v>84</v>
@@ -3788,7 +3827,7 @@
       <c r="V16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="W16" s="25" t="s">
+      <c r="W16" s="23" t="s">
         <v>150</v>
       </c>
       <c r="X16" s="16" t="s">
@@ -3798,7 +3837,7 @@
         <v>83</v>
       </c>
       <c r="Z16" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AA16" s="16" t="s">
         <v>9</v>
@@ -3827,7 +3866,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>9</v>
@@ -3836,34 +3875,34 @@
         <v>51</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J17" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="L17" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>257</v>
       </c>
       <c r="M17" s="16" t="s">
         <v>150</v>
       </c>
       <c r="N17" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="O17" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="O17" s="16" t="s">
-        <v>259</v>
-      </c>
       <c r="P17" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Q17" s="16" t="s">
         <v>83</v>
@@ -3875,7 +3914,7 @@
         <v>83</v>
       </c>
       <c r="T17" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="U17" s="16" t="s">
         <v>84</v>
@@ -3883,7 +3922,7 @@
       <c r="V17" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="W17" s="25" t="s">
+      <c r="W17" s="23" t="s">
         <v>150</v>
       </c>
       <c r="X17" s="16" t="s">
@@ -3893,7 +3932,7 @@
         <v>83</v>
       </c>
       <c r="Z17" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AA17" s="16" t="s">
         <v>9</v>
@@ -3942,196 +3981,196 @@
     <row r="20" spans="1:31" ht="11.25" customHeight="1">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="36"/>
-      <c r="U20" s="36"/>
-      <c r="V20" s="36"/>
-      <c r="W20" s="36"/>
-      <c r="X20" s="36"/>
-      <c r="Y20" s="36"/>
-      <c r="Z20" s="37"/>
-      <c r="AA20" s="33" t="s">
-        <v>230</v>
-      </c>
-      <c r="AB20" s="33" t="s">
+      <c r="F20" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="34"/>
+      <c r="T20" s="34"/>
+      <c r="U20" s="34"/>
+      <c r="V20" s="34"/>
+      <c r="W20" s="34"/>
+      <c r="X20" s="34"/>
+      <c r="Y20" s="34"/>
+      <c r="Z20" s="35"/>
+      <c r="AA20" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="AB20" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC20" s="44"/>
+      <c r="AD20" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="AC20" s="34"/>
-      <c r="AD20" s="33" t="s">
-        <v>235</v>
-      </c>
-      <c r="AE20" s="33" t="s">
-        <v>264</v>
+      <c r="AE20" s="31" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="11.25" customHeight="1">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="39"/>
-      <c r="S21" s="39"/>
-      <c r="T21" s="39"/>
-      <c r="U21" s="39"/>
-      <c r="V21" s="39"/>
-      <c r="W21" s="39"/>
-      <c r="X21" s="39"/>
-      <c r="Y21" s="39"/>
-      <c r="Z21" s="40"/>
-      <c r="AA21" s="33"/>
-      <c r="AB21" s="34"/>
-      <c r="AC21" s="34"/>
-      <c r="AD21" s="33"/>
-      <c r="AE21" s="33"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="37"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="37"/>
+      <c r="U21" s="37"/>
+      <c r="V21" s="37"/>
+      <c r="W21" s="37"/>
+      <c r="X21" s="37"/>
+      <c r="Y21" s="37"/>
+      <c r="Z21" s="38"/>
+      <c r="AA21" s="31"/>
+      <c r="AB21" s="44"/>
+      <c r="AC21" s="44"/>
+      <c r="AD21" s="31"/>
+      <c r="AE21" s="31"/>
     </row>
     <row r="22" spans="1:31" ht="11.25" customHeight="1">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="42"/>
-      <c r="S22" s="42"/>
-      <c r="T22" s="42"/>
-      <c r="U22" s="42"/>
-      <c r="V22" s="42"/>
-      <c r="W22" s="42"/>
-      <c r="X22" s="42"/>
-      <c r="Y22" s="42"/>
-      <c r="Z22" s="43"/>
-      <c r="AA22" s="33"/>
-      <c r="AB22" s="34"/>
-      <c r="AC22" s="34"/>
-      <c r="AD22" s="33"/>
-      <c r="AE22" s="33"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="40"/>
+      <c r="Q22" s="40"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="40"/>
+      <c r="T22" s="40"/>
+      <c r="U22" s="40"/>
+      <c r="V22" s="40"/>
+      <c r="W22" s="40"/>
+      <c r="X22" s="40"/>
+      <c r="Y22" s="40"/>
+      <c r="Z22" s="41"/>
+      <c r="AA22" s="31"/>
+      <c r="AB22" s="44"/>
+      <c r="AC22" s="44"/>
+      <c r="AD22" s="31"/>
+      <c r="AE22" s="31"/>
     </row>
     <row r="23" spans="1:31" ht="11.25" customHeight="1">
       <c r="A23" s="27" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="H23" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="I23" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="C23" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="D23" s="27" t="s">
+      <c r="J23" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="K23" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="L23" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="M23" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="N23" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="O23" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="P23" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q23" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="R23" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="E23" s="27" t="s">
-        <v>266</v>
-      </c>
-      <c r="F23" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="G23" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="H23" s="27" t="s">
+      <c r="S23" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="T23" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="U23" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="V23" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="W23" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="X23" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y23" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="I23" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="J23" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="K23" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="L23" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="M23" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="N23" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="O23" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="P23" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q23" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="R23" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="S23" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="T23" s="27" t="s">
-        <v>190</v>
-      </c>
-      <c r="U23" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="V23" s="27" t="s">
-        <v>244</v>
-      </c>
-      <c r="W23" s="27" t="s">
+      <c r="Z23" s="45" t="s">
         <v>262</v>
       </c>
-      <c r="X23" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="Y23" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="Z23" s="45" t="s">
-        <v>263</v>
-      </c>
       <c r="AA23" s="48" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB23" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="AB23" s="31" t="s">
+      <c r="AC23" s="32" t="s">
         <v>232</v>
       </c>
-      <c r="AC23" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="AD23" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="AE23" s="31" t="s">
-        <v>265</v>
+      <c r="AD23" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="AE23" s="32" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:31">
@@ -4162,10 +4201,10 @@
       <c r="Y24" s="28"/>
       <c r="Z24" s="46"/>
       <c r="AA24" s="48"/>
-      <c r="AB24" s="31"/>
-      <c r="AC24" s="31"/>
-      <c r="AD24" s="31"/>
-      <c r="AE24" s="31"/>
+      <c r="AB24" s="32"/>
+      <c r="AC24" s="32"/>
+      <c r="AD24" s="32"/>
+      <c r="AE24" s="32"/>
     </row>
     <row r="25" spans="1:31">
       <c r="A25" s="28"/>
@@ -4195,10 +4234,10 @@
       <c r="Y25" s="28"/>
       <c r="Z25" s="46"/>
       <c r="AA25" s="48"/>
-      <c r="AB25" s="31"/>
-      <c r="AC25" s="31"/>
-      <c r="AD25" s="31"/>
-      <c r="AE25" s="31"/>
+      <c r="AB25" s="32"/>
+      <c r="AC25" s="32"/>
+      <c r="AD25" s="32"/>
+      <c r="AE25" s="32"/>
     </row>
     <row r="26" spans="1:31">
       <c r="A26" s="29"/>
@@ -4228,10 +4267,10 @@
       <c r="Y26" s="29"/>
       <c r="Z26" s="47"/>
       <c r="AA26" s="48"/>
-      <c r="AB26" s="31"/>
-      <c r="AC26" s="31"/>
-      <c r="AD26" s="31"/>
-      <c r="AE26" s="31"/>
+      <c r="AB26" s="32"/>
+      <c r="AC26" s="32"/>
+      <c r="AD26" s="32"/>
+      <c r="AE26" s="32"/>
     </row>
     <row r="27" spans="1:31">
       <c r="D27" s="1"/>
@@ -4244,9 +4283,9 @@
       <c r="S27" s="2"/>
       <c r="V27" s="2"/>
       <c r="AA27" s="48"/>
-      <c r="AB27" s="31"/>
-      <c r="AC27" s="31"/>
-      <c r="AD27" s="31"/>
+      <c r="AB27" s="32"/>
+      <c r="AC27" s="32"/>
+      <c r="AD27" s="32"/>
     </row>
     <row r="28" spans="1:31">
       <c r="D28" s="1"/>
@@ -4265,9 +4304,9 @@
         <v>170</v>
       </c>
       <c r="AA28" s="48"/>
-      <c r="AB28" s="31"/>
-      <c r="AC28" s="31"/>
-      <c r="AD28" s="32"/>
+      <c r="AB28" s="32"/>
+      <c r="AC28" s="32"/>
+      <c r="AD28" s="43"/>
       <c r="AE28" s="17" t="s">
         <v>170</v>
       </c>
@@ -4277,7 +4316,7 @@
       <c r="E29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" s="1"/>
@@ -4287,7 +4326,7 @@
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
       <c r="X29" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Z29" s="21"/>
       <c r="AA29" s="48"/>
@@ -4300,13 +4339,21 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="AD23:AD28"/>
+    <mergeCell ref="AB20:AC22"/>
+    <mergeCell ref="AD20:AD22"/>
+    <mergeCell ref="W23:W26"/>
+    <mergeCell ref="I23:I26"/>
+    <mergeCell ref="L23:L26"/>
+    <mergeCell ref="J23:J26"/>
+    <mergeCell ref="K23:K26"/>
+    <mergeCell ref="M23:M26"/>
+    <mergeCell ref="Y23:Y26"/>
+    <mergeCell ref="Z23:Z26"/>
+    <mergeCell ref="AA20:AA22"/>
+    <mergeCell ref="AA23:AA29"/>
+    <mergeCell ref="AB23:AB28"/>
     <mergeCell ref="AC23:AC28"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="R23:R26"/>
-    <mergeCell ref="O23:O26"/>
-    <mergeCell ref="V23:V26"/>
-    <mergeCell ref="N23:N26"/>
-    <mergeCell ref="S23:S26"/>
     <mergeCell ref="AE20:AE22"/>
     <mergeCell ref="AE23:AE26"/>
     <mergeCell ref="F20:Z22"/>
@@ -4323,22 +4370,14 @@
     <mergeCell ref="T23:T26"/>
     <mergeCell ref="U23:U26"/>
     <mergeCell ref="B23:B26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="R23:R26"/>
+    <mergeCell ref="O23:O26"/>
+    <mergeCell ref="V23:V26"/>
+    <mergeCell ref="N23:N26"/>
+    <mergeCell ref="S23:S26"/>
     <mergeCell ref="E23:E26"/>
-    <mergeCell ref="AD23:AD28"/>
-    <mergeCell ref="AB20:AC22"/>
-    <mergeCell ref="AD20:AD22"/>
-    <mergeCell ref="W23:W26"/>
-    <mergeCell ref="I23:I26"/>
-    <mergeCell ref="L23:L26"/>
-    <mergeCell ref="J23:J26"/>
-    <mergeCell ref="K23:K26"/>
-    <mergeCell ref="M23:M26"/>
     <mergeCell ref="H23:H26"/>
-    <mergeCell ref="Y23:Y26"/>
-    <mergeCell ref="Z23:Z26"/>
-    <mergeCell ref="AA20:AA22"/>
-    <mergeCell ref="AA23:AA29"/>
-    <mergeCell ref="AB23:AB28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4348,12 +4387,12 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
+    <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A2:AB32"/>
+  <dimension ref="A2:AB66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -4362,7 +4401,7 @@
     <col min="2" max="2" width="22.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="24" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="19" style="2" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" style="2" customWidth="1"/>
@@ -4373,10 +4412,10 @@
     <col min="13" max="13" width="34" style="2" customWidth="1"/>
     <col min="14" max="14" width="35.140625" style="2" customWidth="1"/>
     <col min="15" max="15" width="36.42578125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="25.42578125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="35.28515625" style="2" customWidth="1"/>
     <col min="17" max="17" width="33.140625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="28.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="28.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="36.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="39" style="1" customWidth="1"/>
     <col min="20" max="20" width="30.42578125" style="1" customWidth="1"/>
     <col min="21" max="21" width="31.28515625" style="2" customWidth="1"/>
     <col min="22" max="22" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -4384,9 +4423,10 @@
     <col min="24" max="24" width="43.140625" style="1" customWidth="1"/>
     <col min="25" max="25" width="42.140625" style="1" customWidth="1"/>
     <col min="26" max="26" width="25.5703125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="22.42578125" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="1"/>
+    <col min="27" max="27" width="25.28515625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="41.42578125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="26" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:28" ht="21">
@@ -4404,18 +4444,18 @@
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="3" t="s">
-        <v>172</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="21">
-      <c r="A4" s="44" t="s">
-        <v>185</v>
-      </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="A4" s="42" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="19"/>
@@ -4444,40 +4484,40 @@
         <v>56</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="P7" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Q7" s="14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="R7" s="14" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="S7" s="14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="T7" s="14" t="s">
         <v>110</v>
@@ -4495,1111 +4535,1149 @@
         <v>120</v>
       </c>
       <c r="Y7" s="14" t="s">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="Z7" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AA7" s="14" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="AB7" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28">
-      <c r="A8" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" s="13" customFormat="1">
+      <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="16" t="s">
+      <c r="E8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="H8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="H8" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="I8" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="J8" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="K8" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="M8" s="16" t="s">
+      <c r="L8" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="N8" s="16" t="s">
+      <c r="M8" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="O8" s="16" t="s">
+      <c r="N8" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="P8" s="16" t="s">
+      <c r="O8" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="P8" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="Q8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="S8" s="16" t="s">
+      <c r="R8" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="T8" s="16" t="s">
+      <c r="S8" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="T8" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="U8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="V8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="W8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="X8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y8" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB8" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28">
-      <c r="A9" s="2" t="s">
+      <c r="U8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="V8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="W8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="X8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB8" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" s="13" customFormat="1">
+      <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="16" t="s">
+      <c r="E9" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="H9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="2" t="s">
+      <c r="H9" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="I9" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="J9" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="K9" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="L9" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="N9" s="16" t="s">
+      <c r="M9" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="N9" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="O9" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="P9" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="R9" s="2" t="s">
+      <c r="Q9" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="S9" s="16" t="s">
+      <c r="R9" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="T9" s="16" t="s">
+      <c r="S9" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="T9" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="U9" s="16" t="s">
+      <c r="U9" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="V9" s="16" t="s">
+      <c r="V9" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="W9" s="16" t="s">
+      <c r="W9" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="X9" s="16" t="s">
+      <c r="X9" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="Y9" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB9" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28">
-      <c r="A10" s="2" t="s">
+      <c r="Y9" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z9" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA9" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB9" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" s="13" customFormat="1">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="16" t="s">
+      <c r="E10" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L10" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="N10" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R10" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="S10" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="T10" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="U10" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="V10" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="W10" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="X10" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y10" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z10" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA10" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB10" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="I10" s="23" t="s">
+    </row>
+    <row r="11" spans="1:28" s="13" customFormat="1">
+      <c r="A11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="J10" s="23" t="s">
+      <c r="I11" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="K10" s="23" t="s">
+      <c r="J11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="L10" s="23" t="s">
+      <c r="K11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="M10" s="24" t="s">
+      <c r="L11" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="N10" s="24" t="s">
+      <c r="M11" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="O10" s="16" t="s">
+      <c r="N11" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="P10" s="24" t="s">
+      <c r="O11" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="Q10" s="23" t="s">
+      <c r="P11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="R10" s="23" t="s">
+      <c r="R11" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="S11" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="T11" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="U11" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="V11" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="W11" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="X11" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y11" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z11" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA11" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB11" s="23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" s="13" customFormat="1">
+      <c r="A12" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="N12" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O12" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P12" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="S10" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="T10" s="24" t="s">
+      <c r="Q12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" s="23" t="s">
+        <v>268</v>
+      </c>
+      <c r="S12" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="T12" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="U12" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="V12" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="W12" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="X12" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y12" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z12" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA12" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB12" s="23" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" s="13" customFormat="1">
+      <c r="A13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="N13" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O13" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="P13" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" s="23" t="s">
+        <v>271</v>
+      </c>
+      <c r="S13" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="T13" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="U13" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="V13" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="W13" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="X13" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB13" s="23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" s="13" customFormat="1">
+      <c r="A14" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="N14" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O14" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" s="23" t="s">
+        <v>271</v>
+      </c>
+      <c r="S14" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="T14" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="U14" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="V14" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="W14" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="X14" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y14" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z14" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA14" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB14" s="23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" s="13" customFormat="1">
+      <c r="A15" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L15" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M15" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="N15" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="P15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="S15" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="T15" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="U15" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="V15" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="W15" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="X15" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="Y15" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z15" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA15" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB15" s="23" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" s="13" customFormat="1">
+      <c r="A16" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L16" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="N16" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O16" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="P16" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R16" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="S16" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="T16" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="U10" s="24" t="s">
+      <c r="U16" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="V16" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="W16" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="X16" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="Y16" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z16" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA16" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB16" s="23" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" s="13" customFormat="1">
+      <c r="A17" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="N17" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="P17" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="V10" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="W10" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="X10" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y10" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB10" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28">
-      <c r="A11" s="2" t="s">
+      <c r="R17" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="S17" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="T17" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="U17" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="V17" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="W17" s="23" t="s">
+        <v>281</v>
+      </c>
+      <c r="X17" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="Y17" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z17" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA17" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB17" s="23" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" s="12" customFormat="1">
+      <c r="A18" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B18" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C18" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D18" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="J11" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="K11" s="23" t="s">
+      <c r="E18" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="L11" s="23" t="s">
+      <c r="L18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="M11" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="N11" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="O11" s="16" t="s">
+      <c r="R18" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="S18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="T18" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="U18" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="P11" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="R11" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="S11" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="T11" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="U11" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="V11" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="W11" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="X11" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y11" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z11" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA11" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB11" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28">
-      <c r="A12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>270</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>271</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="L12" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="M12" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="N12" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="O12" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="P12" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="R12" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="S12" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="T12" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="U12" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="V12" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="W12" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="X12" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y12" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z12" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA12" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB12" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>273</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="I13" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="J13" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="K13" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="L13" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="M13" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="N13" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="O13" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="P13" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="R13" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="S13" s="24" t="s">
-        <v>272</v>
-      </c>
-      <c r="T13" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="U13" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="V13" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="W13" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="X13" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB13" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28">
-      <c r="A14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>273</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="K14" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="L14" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="M14" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="N14" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="O14" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="P14" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="R14" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="S14" s="24" t="s">
-        <v>272</v>
-      </c>
-      <c r="T14" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="U14" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="V14" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="W14" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="X14" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y14" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z14" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA14" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB14" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28">
-      <c r="A15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="16" t="s">
+      <c r="V18" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="W18" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="X18" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="Y18" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z18" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA18" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB18" s="12" t="s">
         <v>275</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>276</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M15" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="N15" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="O15" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P15" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S15" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="T15" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="U15" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="V15" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="W15" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="X15" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="Y15" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z15" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA15" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="AB15" s="16" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28">
-      <c r="A16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>278</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>276</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M16" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="N16" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="O16" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="P16" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S16" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="T16" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="U16" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="V16" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="W16" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="X16" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="Y16" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z16" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA16" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="AB16" s="16" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28">
-      <c r="A17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>281</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>276</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="N17" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="O17" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="P17" s="16" t="s">
-        <v>279</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="S17" s="16" t="s">
-        <v>280</v>
-      </c>
-      <c r="T17" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="U17" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="V17" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="W17" s="16" t="s">
-        <v>282</v>
-      </c>
-      <c r="X17" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="Y17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z17" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA17" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB17" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" s="2" customFormat="1">
-      <c r="A18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="T18" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="U18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V18" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="W18" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="X18" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="Y18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB18" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:28" s="2" customFormat="1"/>
     <row r="20" spans="1:28">
       <c r="E20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
       <c r="K20" s="2"/>
+      <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="1"/>
       <c r="X20" s="2"/>
-      <c r="Y20" s="2"/>
     </row>
     <row r="21" spans="1:28" ht="11.25" customHeight="1">
-      <c r="E21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="K21" s="2"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="1"/>
-      <c r="X21" s="2"/>
-      <c r="Z21" s="33" t="s">
+      <c r="E21" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="31"/>
+      <c r="S21" s="31"/>
+      <c r="T21" s="31"/>
+      <c r="U21" s="31"/>
+      <c r="V21" s="31"/>
+      <c r="W21" s="31"/>
+      <c r="X21" s="31"/>
+      <c r="Y21" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="Z21" s="31"/>
+      <c r="AA21" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="AA21" s="33"/>
-      <c r="AB21" s="33" t="s">
-        <v>235</v>
+      <c r="AB21" s="31" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="22" spans="1:28">
-      <c r="E22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="K22" s="2"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="1"/>
-      <c r="X22" s="2"/>
-      <c r="Z22" s="33"/>
-      <c r="AA22" s="33"/>
-      <c r="AB22" s="33"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="31"/>
+      <c r="W22" s="31"/>
+      <c r="X22" s="31"/>
+      <c r="Y22" s="31"/>
+      <c r="Z22" s="31"/>
+      <c r="AA22" s="31"/>
+      <c r="AB22" s="31" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="23" spans="1:28">
-      <c r="E23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="K23" s="2"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="1"/>
-      <c r="X23" s="2"/>
-      <c r="Z23" s="33"/>
-      <c r="AA23" s="33"/>
-      <c r="AB23" s="33"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="31"/>
+      <c r="S23" s="31"/>
+      <c r="T23" s="31"/>
+      <c r="U23" s="31"/>
+      <c r="V23" s="31"/>
+      <c r="W23" s="31"/>
+      <c r="X23" s="31"/>
+      <c r="Y23" s="31"/>
+      <c r="Z23" s="31"/>
+      <c r="AA23" s="31"/>
+      <c r="AB23" s="31"/>
     </row>
     <row r="24" spans="1:28" ht="11.25" customHeight="1">
       <c r="A24" s="27" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C24" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="G24" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="H24" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="J24" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="D24" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="E24" s="27" t="s">
-        <v>266</v>
-      </c>
-      <c r="F24" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="G24" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="J24" s="27" t="s">
-        <v>192</v>
-      </c>
       <c r="K24" s="27" t="s">
-        <v>176</v>
+        <v>285</v>
       </c>
       <c r="L24" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="M24" s="27" t="s">
+      <c r="M24" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="N24" s="52" t="s">
+        <v>291</v>
+      </c>
+      <c r="O24" s="53" t="s">
+        <v>298</v>
+      </c>
+      <c r="P24" s="27" t="s">
+        <v>299</v>
+      </c>
+      <c r="Q24" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="R24" s="27" t="s">
         <v>287</v>
       </c>
-      <c r="N24" s="31" t="s">
-        <v>298</v>
-      </c>
-      <c r="O24" s="55" t="s">
+      <c r="S24" s="27" t="s">
+        <v>303</v>
+      </c>
+      <c r="T24" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="U24" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="V24" s="27" t="s">
         <v>292</v>
       </c>
-      <c r="P24" s="56" t="s">
-        <v>299</v>
-      </c>
-      <c r="Q24" s="27" t="s">
-        <v>300</v>
-      </c>
-      <c r="R24" s="27" t="s">
-        <v>284</v>
-      </c>
-      <c r="S24" s="27" t="s">
-        <v>288</v>
-      </c>
-      <c r="T24" s="27" t="s">
-        <v>289</v>
-      </c>
-      <c r="U24" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="V24" s="27" t="s">
+      <c r="W24" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="W24" s="27" t="s">
+      <c r="X24" s="27" t="s">
         <v>294</v>
       </c>
-      <c r="X24" s="27" t="s">
+      <c r="Y24" s="56" t="s">
         <v>295</v>
       </c>
-      <c r="Y24" s="2"/>
-      <c r="Z24" s="49" t="s">
+      <c r="Z24" s="59" t="s">
         <v>296</v>
       </c>
-      <c r="AA24" s="52" t="s">
-        <v>297</v>
-      </c>
-      <c r="AB24" s="31" t="s">
-        <v>236</v>
+      <c r="AA24" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="AB24" s="49" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="25" spans="1:28">
@@ -5610,15 +5688,15 @@
       <c r="E25" s="28"/>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
-      <c r="H25" s="1"/>
+      <c r="H25" s="28"/>
       <c r="I25" s="28"/>
       <c r="J25" s="28"/>
       <c r="K25" s="28"/>
       <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="55"/>
-      <c r="P25" s="57"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="52"/>
+      <c r="O25" s="54"/>
+      <c r="P25" s="28"/>
       <c r="Q25" s="28"/>
       <c r="R25" s="28"/>
       <c r="S25" s="28"/>
@@ -5627,10 +5705,10 @@
       <c r="V25" s="28"/>
       <c r="W25" s="28"/>
       <c r="X25" s="28"/>
-      <c r="Y25" s="2"/>
-      <c r="Z25" s="50"/>
-      <c r="AA25" s="53"/>
-      <c r="AB25" s="31"/>
+      <c r="Y25" s="57"/>
+      <c r="Z25" s="60"/>
+      <c r="AA25" s="32"/>
+      <c r="AB25" s="50"/>
     </row>
     <row r="26" spans="1:28">
       <c r="A26" s="28"/>
@@ -5640,15 +5718,15 @@
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
-      <c r="H26" s="1"/>
+      <c r="H26" s="28"/>
       <c r="I26" s="28"/>
       <c r="J26" s="28"/>
       <c r="K26" s="28"/>
       <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="55"/>
-      <c r="P26" s="57"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="52"/>
+      <c r="O26" s="54"/>
+      <c r="P26" s="28"/>
       <c r="Q26" s="28"/>
       <c r="R26" s="28"/>
       <c r="S26" s="28"/>
@@ -5657,10 +5735,10 @@
       <c r="V26" s="28"/>
       <c r="W26" s="28"/>
       <c r="X26" s="28"/>
-      <c r="Y26" s="2"/>
-      <c r="Z26" s="50"/>
-      <c r="AA26" s="53"/>
-      <c r="AB26" s="31"/>
+      <c r="Y26" s="57"/>
+      <c r="Z26" s="60"/>
+      <c r="AA26" s="32"/>
+      <c r="AB26" s="50"/>
     </row>
     <row r="27" spans="1:28">
       <c r="A27" s="29"/>
@@ -5670,15 +5748,15 @@
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
       <c r="G27" s="29"/>
-      <c r="H27" s="1"/>
+      <c r="H27" s="29"/>
       <c r="I27" s="29"/>
       <c r="J27" s="29"/>
       <c r="K27" s="29"/>
       <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="31"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="52"/>
       <c r="O27" s="55"/>
-      <c r="P27" s="58"/>
+      <c r="P27" s="29"/>
       <c r="Q27" s="29"/>
       <c r="R27" s="29"/>
       <c r="S27" s="29"/>
@@ -5687,79 +5765,78 @@
       <c r="V27" s="29"/>
       <c r="W27" s="29"/>
       <c r="X27" s="29"/>
-      <c r="Y27" s="2"/>
-      <c r="Z27" s="50"/>
-      <c r="AA27" s="53"/>
-      <c r="AB27" s="31"/>
+      <c r="Y27" s="57"/>
+      <c r="Z27" s="60"/>
+      <c r="AA27" s="32"/>
+      <c r="AB27" s="50"/>
     </row>
     <row r="28" spans="1:28">
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="H28" s="1"/>
       <c r="K28" s="2"/>
+      <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="55"/>
+      <c r="N28" s="52"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
       <c r="U28" s="1"/>
       <c r="X28" s="2"/>
-      <c r="Y28" s="2"/>
-      <c r="Z28" s="50"/>
-      <c r="AA28" s="53"/>
-      <c r="AB28" s="31"/>
+      <c r="Y28" s="57"/>
+      <c r="Z28" s="60"/>
+      <c r="AA28" s="32"/>
+      <c r="AB28" s="50"/>
     </row>
     <row r="29" spans="1:28">
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="J29" s="17" t="s">
+        <v>170</v>
+      </c>
       <c r="K29" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="L29" s="17" t="s">
-        <v>170</v>
-      </c>
+      <c r="L29" s="1"/>
       <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="55"/>
+      <c r="N29" s="52"/>
       <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
+      <c r="S29" s="17" t="s">
+        <v>304</v>
+      </c>
       <c r="U29" s="17" t="s">
         <v>170</v>
       </c>
       <c r="X29" s="2"/>
-      <c r="Y29" s="2"/>
-      <c r="Z29" s="51"/>
-      <c r="AA29" s="54"/>
-      <c r="AB29" s="31"/>
-    </row>
-    <row r="30" spans="1:28" ht="180">
+      <c r="Y29" s="58"/>
+      <c r="Z29" s="61"/>
+      <c r="AA29" s="32"/>
+      <c r="AB29" s="51"/>
+    </row>
+    <row r="30" spans="1:28" ht="202.5">
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="K30" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="L30" s="26" t="s">
-        <v>285</v>
-      </c>
+      <c r="J30" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="K30" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="L30" s="1"/>
       <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="55"/>
+      <c r="N30" s="52"/>
       <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
+      <c r="S30" s="25" t="s">
+        <v>305</v>
+      </c>
       <c r="U30" s="20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="X30" s="2"/>
-      <c r="Y30" s="2"/>
     </row>
     <row r="31" spans="1:28">
       <c r="E31" s="1"/>
       <c r="K31" s="2"/>
       <c r="L31" s="1"/>
-      <c r="R31" s="2"/>
       <c r="U31" s="1"/>
       <c r="V31" s="2"/>
     </row>
@@ -5767,43 +5844,214 @@
       <c r="E32" s="1"/>
       <c r="K32" s="2"/>
       <c r="L32" s="1"/>
-      <c r="R32" s="2"/>
-      <c r="U32" s="1"/>
-      <c r="V32" s="2"/>
+    </row>
+    <row r="33" spans="17:21">
+      <c r="Q33" s="1"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="1"/>
+    </row>
+    <row r="34" spans="17:21">
+      <c r="Q34" s="1"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="1"/>
+    </row>
+    <row r="35" spans="17:21">
+      <c r="Q35" s="1"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="1"/>
+    </row>
+    <row r="36" spans="17:21">
+      <c r="Q36" s="1"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="1"/>
+    </row>
+    <row r="37" spans="17:21">
+      <c r="Q37" s="1"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="1"/>
+    </row>
+    <row r="38" spans="17:21">
+      <c r="Q38" s="1"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="1"/>
+    </row>
+    <row r="39" spans="17:21">
+      <c r="Q39" s="1"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="1"/>
+    </row>
+    <row r="40" spans="17:21">
+      <c r="Q40" s="1"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="1"/>
+    </row>
+    <row r="41" spans="17:21">
+      <c r="Q41" s="1"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="1"/>
+    </row>
+    <row r="42" spans="17:21">
+      <c r="Q42" s="1"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="1"/>
+    </row>
+    <row r="43" spans="17:21">
+      <c r="Q43" s="1"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="1"/>
+    </row>
+    <row r="44" spans="17:21">
+      <c r="Q44" s="1"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="1"/>
+    </row>
+    <row r="45" spans="17:21">
+      <c r="Q45" s="1"/>
+      <c r="T45" s="2"/>
+      <c r="U45" s="1"/>
+    </row>
+    <row r="46" spans="17:21">
+      <c r="Q46" s="1"/>
+      <c r="T46" s="2"/>
+      <c r="U46" s="1"/>
+    </row>
+    <row r="47" spans="17:21">
+      <c r="Q47" s="1"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="1"/>
+    </row>
+    <row r="48" spans="17:21">
+      <c r="Q48" s="1"/>
+      <c r="T48" s="2"/>
+      <c r="U48" s="1"/>
+    </row>
+    <row r="49" spans="17:21">
+      <c r="Q49" s="1"/>
+      <c r="T49" s="2"/>
+      <c r="U49" s="1"/>
+    </row>
+    <row r="50" spans="17:21">
+      <c r="Q50" s="1"/>
+      <c r="T50" s="2"/>
+      <c r="U50" s="1"/>
+    </row>
+    <row r="51" spans="17:21">
+      <c r="Q51" s="1"/>
+      <c r="T51" s="2"/>
+      <c r="U51" s="1"/>
+    </row>
+    <row r="52" spans="17:21">
+      <c r="Q52" s="1"/>
+      <c r="T52" s="2"/>
+      <c r="U52" s="1"/>
+    </row>
+    <row r="53" spans="17:21">
+      <c r="Q53" s="1"/>
+      <c r="T53" s="2"/>
+      <c r="U53" s="1"/>
+    </row>
+    <row r="54" spans="17:21">
+      <c r="Q54" s="1"/>
+      <c r="T54" s="2"/>
+      <c r="U54" s="1"/>
+    </row>
+    <row r="55" spans="17:21">
+      <c r="Q55" s="1"/>
+      <c r="T55" s="2"/>
+      <c r="U55" s="1"/>
+    </row>
+    <row r="56" spans="17:21">
+      <c r="Q56" s="1"/>
+      <c r="T56" s="2"/>
+      <c r="U56" s="1"/>
+    </row>
+    <row r="57" spans="17:21">
+      <c r="Q57" s="1"/>
+      <c r="T57" s="2"/>
+      <c r="U57" s="1"/>
+    </row>
+    <row r="58" spans="17:21">
+      <c r="Q58" s="1"/>
+      <c r="T58" s="2"/>
+      <c r="U58" s="1"/>
+    </row>
+    <row r="59" spans="17:21">
+      <c r="Q59" s="1"/>
+      <c r="T59" s="2"/>
+      <c r="U59" s="1"/>
+    </row>
+    <row r="60" spans="17:21">
+      <c r="Q60" s="1"/>
+      <c r="T60" s="2"/>
+      <c r="U60" s="1"/>
+    </row>
+    <row r="61" spans="17:21">
+      <c r="Q61" s="1"/>
+      <c r="T61" s="2"/>
+      <c r="U61" s="1"/>
+    </row>
+    <row r="62" spans="17:21">
+      <c r="Q62" s="1"/>
+      <c r="T62" s="2"/>
+      <c r="U62" s="1"/>
+    </row>
+    <row r="63" spans="17:21">
+      <c r="Q63" s="1"/>
+      <c r="T63" s="2"/>
+      <c r="U63" s="1"/>
+    </row>
+    <row r="64" spans="17:21">
+      <c r="Q64" s="1"/>
+      <c r="T64" s="2"/>
+      <c r="U64" s="1"/>
+    </row>
+    <row r="65" spans="17:21">
+      <c r="Q65" s="1"/>
+      <c r="T65" s="2"/>
+      <c r="U65" s="1"/>
+    </row>
+    <row r="66" spans="17:21">
+      <c r="Q66" s="1"/>
+      <c r="T66" s="2"/>
+      <c r="U66" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="E24:E27"/>
+  <mergeCells count="35">
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="X24:X27"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="N24:N30"/>
+    <mergeCell ref="T24:T27"/>
+    <mergeCell ref="U24:U27"/>
+    <mergeCell ref="M24:M27"/>
+    <mergeCell ref="P24:P27"/>
+    <mergeCell ref="Q24:Q27"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="L24:L27"/>
+    <mergeCell ref="R24:R27"/>
+    <mergeCell ref="G24:G27"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="P24:P27"/>
+    <mergeCell ref="AB21:AB23"/>
+    <mergeCell ref="AB24:AB29"/>
+    <mergeCell ref="S24:S27"/>
+    <mergeCell ref="E21:X23"/>
     <mergeCell ref="V24:V27"/>
     <mergeCell ref="W24:W27"/>
-    <mergeCell ref="X24:X27"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="O24:O30"/>
-    <mergeCell ref="T24:T27"/>
-    <mergeCell ref="U24:U27"/>
-    <mergeCell ref="N24:N27"/>
-    <mergeCell ref="Q24:Q27"/>
-    <mergeCell ref="R24:R27"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="L24:L27"/>
-    <mergeCell ref="M24:M27"/>
-    <mergeCell ref="S24:S27"/>
-    <mergeCell ref="Z21:AA23"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="O24:O27"/>
+    <mergeCell ref="Y21:Z23"/>
+    <mergeCell ref="Y24:Y29"/>
     <mergeCell ref="Z24:Z29"/>
     <mergeCell ref="AA24:AA29"/>
-    <mergeCell ref="AB24:AB29"/>
-    <mergeCell ref="AB21:AB23"/>
+    <mergeCell ref="AA21:AA23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5815,10 +6063,10 @@
   <sheetPr>
     <tabColor rgb="FFFA7E7E"/>
   </sheetPr>
-  <dimension ref="A2:H16"/>
+  <dimension ref="A2:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -6134,6 +6382,11 @@
       </c>
       <c r="H16" s="2" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
+      <c r="E19" s="2" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de Conferência LN - DEV e CAR
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_CAR.xlsx
+++ b/Documentação/Planilhas/Conferencia_CAR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="93" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="319">
   <si>
     <t>1</t>
   </si>
@@ -1032,6 +1032,15 @@
   </si>
   <si>
     <t>tfcmg4501m000, tfacr2520m000</t>
+  </si>
+  <si>
+    <t>Sessão tfcmg4521m000</t>
+  </si>
+  <si>
+    <t>Não tenho permissão  de acesso</t>
+  </si>
+  <si>
+    <t>Pegar a informação do Lote Criado em</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1094,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1113,6 +1122,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA7E7E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1368,7 +1383,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1446,11 +1461,29 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1482,22 +1515,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1536,8 +1554,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1548,8 +1575,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFA7E7E"/>
       <color rgb="FFFFFFCC"/>
-      <color rgb="FFFA7E7E"/>
       <color rgb="FFCCECFF"/>
       <color rgb="FFFF5050"/>
     </mruColors>
@@ -1918,7 +1945,7 @@
   </sheetPr>
   <dimension ref="A2:AG22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -2345,17 +2372,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
     <mergeCell ref="I19:I22"/>
     <mergeCell ref="D19:D22"/>
     <mergeCell ref="E19:E22"/>
     <mergeCell ref="F19:F22"/>
     <mergeCell ref="G19:G22"/>
     <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2917,14 +2944,14 @@
       </c>
     </row>
     <row r="4" spans="1:31" ht="21">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
       <c r="G4" s="1"/>
       <c r="P4" s="19"/>
       <c r="AB4" s="2"/>
@@ -4005,102 +4032,102 @@
     <row r="20" spans="1:31" ht="11.25" customHeight="1">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="34"/>
-      <c r="T20" s="34"/>
-      <c r="U20" s="34"/>
-      <c r="V20" s="34"/>
-      <c r="W20" s="34"/>
-      <c r="X20" s="34"/>
-      <c r="Y20" s="34"/>
-      <c r="Z20" s="35"/>
-      <c r="AA20" s="31" t="s">
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40"/>
+      <c r="U20" s="40"/>
+      <c r="V20" s="40"/>
+      <c r="W20" s="40"/>
+      <c r="X20" s="40"/>
+      <c r="Y20" s="40"/>
+      <c r="Z20" s="41"/>
+      <c r="AA20" s="33" t="s">
         <v>229</v>
       </c>
-      <c r="AB20" s="31" t="s">
+      <c r="AB20" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="AC20" s="44"/>
-      <c r="AD20" s="31" t="s">
+      <c r="AC20" s="34"/>
+      <c r="AD20" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="AE20" s="31" t="s">
+      <c r="AE20" s="33" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="11.25" customHeight="1">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="37"/>
-      <c r="Q21" s="37"/>
-      <c r="R21" s="37"/>
-      <c r="S21" s="37"/>
-      <c r="T21" s="37"/>
-      <c r="U21" s="37"/>
-      <c r="V21" s="37"/>
-      <c r="W21" s="37"/>
-      <c r="X21" s="37"/>
-      <c r="Y21" s="37"/>
-      <c r="Z21" s="38"/>
-      <c r="AA21" s="31"/>
-      <c r="AB21" s="44"/>
-      <c r="AC21" s="44"/>
-      <c r="AD21" s="31"/>
-      <c r="AE21" s="31"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="43"/>
+      <c r="S21" s="43"/>
+      <c r="T21" s="43"/>
+      <c r="U21" s="43"/>
+      <c r="V21" s="43"/>
+      <c r="W21" s="43"/>
+      <c r="X21" s="43"/>
+      <c r="Y21" s="43"/>
+      <c r="Z21" s="44"/>
+      <c r="AA21" s="33"/>
+      <c r="AB21" s="34"/>
+      <c r="AC21" s="34"/>
+      <c r="AD21" s="33"/>
+      <c r="AE21" s="33"/>
     </row>
     <row r="22" spans="1:31" ht="11.25" customHeight="1">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="40"/>
-      <c r="P22" s="40"/>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="40"/>
-      <c r="S22" s="40"/>
-      <c r="T22" s="40"/>
-      <c r="U22" s="40"/>
-      <c r="V22" s="40"/>
-      <c r="W22" s="40"/>
-      <c r="X22" s="40"/>
-      <c r="Y22" s="40"/>
-      <c r="Z22" s="41"/>
-      <c r="AA22" s="31"/>
-      <c r="AB22" s="44"/>
-      <c r="AC22" s="44"/>
-      <c r="AD22" s="31"/>
-      <c r="AE22" s="31"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="46"/>
+      <c r="Q22" s="46"/>
+      <c r="R22" s="46"/>
+      <c r="S22" s="46"/>
+      <c r="T22" s="46"/>
+      <c r="U22" s="46"/>
+      <c r="V22" s="46"/>
+      <c r="W22" s="46"/>
+      <c r="X22" s="46"/>
+      <c r="Y22" s="46"/>
+      <c r="Z22" s="47"/>
+      <c r="AA22" s="33"/>
+      <c r="AB22" s="34"/>
+      <c r="AC22" s="34"/>
+      <c r="AD22" s="33"/>
+      <c r="AE22" s="33"/>
     </row>
     <row r="23" spans="1:31" ht="11.25" customHeight="1">
       <c r="A23" s="27" t="s">
@@ -4178,22 +4205,22 @@
       <c r="Y23" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="Z23" s="45" t="s">
+      <c r="Z23" s="35" t="s">
         <v>262</v>
       </c>
-      <c r="AA23" s="48" t="s">
+      <c r="AA23" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="AB23" s="32" t="s">
+      <c r="AB23" s="31" t="s">
         <v>231</v>
       </c>
-      <c r="AC23" s="32" t="s">
+      <c r="AC23" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="AD23" s="32" t="s">
+      <c r="AD23" s="31" t="s">
         <v>235</v>
       </c>
-      <c r="AE23" s="32" t="s">
+      <c r="AE23" s="31" t="s">
         <v>264</v>
       </c>
     </row>
@@ -4223,12 +4250,12 @@
       <c r="W24" s="28"/>
       <c r="X24" s="28"/>
       <c r="Y24" s="28"/>
-      <c r="Z24" s="46"/>
-      <c r="AA24" s="48"/>
-      <c r="AB24" s="32"/>
-      <c r="AC24" s="32"/>
-      <c r="AD24" s="32"/>
-      <c r="AE24" s="32"/>
+      <c r="Z24" s="36"/>
+      <c r="AA24" s="38"/>
+      <c r="AB24" s="31"/>
+      <c r="AC24" s="31"/>
+      <c r="AD24" s="31"/>
+      <c r="AE24" s="31"/>
     </row>
     <row r="25" spans="1:31">
       <c r="A25" s="28"/>
@@ -4256,12 +4283,12 @@
       <c r="W25" s="28"/>
       <c r="X25" s="28"/>
       <c r="Y25" s="28"/>
-      <c r="Z25" s="46"/>
-      <c r="AA25" s="48"/>
-      <c r="AB25" s="32"/>
-      <c r="AC25" s="32"/>
-      <c r="AD25" s="32"/>
-      <c r="AE25" s="32"/>
+      <c r="Z25" s="36"/>
+      <c r="AA25" s="38"/>
+      <c r="AB25" s="31"/>
+      <c r="AC25" s="31"/>
+      <c r="AD25" s="31"/>
+      <c r="AE25" s="31"/>
     </row>
     <row r="26" spans="1:31">
       <c r="A26" s="29"/>
@@ -4289,12 +4316,12 @@
       <c r="W26" s="29"/>
       <c r="X26" s="29"/>
       <c r="Y26" s="29"/>
-      <c r="Z26" s="47"/>
-      <c r="AA26" s="48"/>
-      <c r="AB26" s="32"/>
-      <c r="AC26" s="32"/>
-      <c r="AD26" s="32"/>
-      <c r="AE26" s="32"/>
+      <c r="Z26" s="37"/>
+      <c r="AA26" s="38"/>
+      <c r="AB26" s="31"/>
+      <c r="AC26" s="31"/>
+      <c r="AD26" s="31"/>
+      <c r="AE26" s="31"/>
     </row>
     <row r="27" spans="1:31">
       <c r="D27" s="1"/>
@@ -4306,10 +4333,10 @@
       <c r="R27" s="1"/>
       <c r="S27" s="2"/>
       <c r="V27" s="2"/>
-      <c r="AA27" s="48"/>
-      <c r="AB27" s="32"/>
-      <c r="AC27" s="32"/>
-      <c r="AD27" s="32"/>
+      <c r="AA27" s="38"/>
+      <c r="AB27" s="31"/>
+      <c r="AC27" s="31"/>
+      <c r="AD27" s="31"/>
     </row>
     <row r="28" spans="1:31">
       <c r="D28" s="1"/>
@@ -4327,10 +4354,10 @@
       <c r="X28" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="AA28" s="48"/>
-      <c r="AB28" s="32"/>
-      <c r="AC28" s="32"/>
-      <c r="AD28" s="43"/>
+      <c r="AA28" s="38"/>
+      <c r="AB28" s="31"/>
+      <c r="AC28" s="31"/>
+      <c r="AD28" s="32"/>
       <c r="AE28" s="17" t="s">
         <v>170</v>
       </c>
@@ -4353,7 +4380,7 @@
         <v>186</v>
       </c>
       <c r="Z29" s="21"/>
-      <c r="AA29" s="48"/>
+      <c r="AA29" s="38"/>
       <c r="AB29" s="22"/>
       <c r="AC29" s="2"/>
       <c r="AD29" s="2"/>
@@ -4363,21 +4390,14 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="AD23:AD28"/>
-    <mergeCell ref="AB20:AC22"/>
-    <mergeCell ref="AD20:AD22"/>
-    <mergeCell ref="W23:W26"/>
-    <mergeCell ref="I23:I26"/>
-    <mergeCell ref="L23:L26"/>
-    <mergeCell ref="J23:J26"/>
-    <mergeCell ref="K23:K26"/>
-    <mergeCell ref="M23:M26"/>
-    <mergeCell ref="Y23:Y26"/>
-    <mergeCell ref="Z23:Z26"/>
-    <mergeCell ref="AA20:AA22"/>
-    <mergeCell ref="AA23:AA29"/>
-    <mergeCell ref="AB23:AB28"/>
-    <mergeCell ref="AC23:AC28"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="R23:R26"/>
+    <mergeCell ref="O23:O26"/>
+    <mergeCell ref="V23:V26"/>
+    <mergeCell ref="N23:N26"/>
+    <mergeCell ref="S23:S26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="H23:H26"/>
     <mergeCell ref="AE20:AE22"/>
     <mergeCell ref="AE23:AE26"/>
     <mergeCell ref="F20:Z22"/>
@@ -4394,14 +4414,21 @@
     <mergeCell ref="T23:T26"/>
     <mergeCell ref="U23:U26"/>
     <mergeCell ref="B23:B26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="R23:R26"/>
-    <mergeCell ref="O23:O26"/>
-    <mergeCell ref="V23:V26"/>
-    <mergeCell ref="N23:N26"/>
-    <mergeCell ref="S23:S26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="AD23:AD28"/>
+    <mergeCell ref="AB20:AC22"/>
+    <mergeCell ref="AD20:AD22"/>
+    <mergeCell ref="W23:W26"/>
+    <mergeCell ref="I23:I26"/>
+    <mergeCell ref="L23:L26"/>
+    <mergeCell ref="J23:J26"/>
+    <mergeCell ref="K23:K26"/>
+    <mergeCell ref="M23:M26"/>
+    <mergeCell ref="Y23:Y26"/>
+    <mergeCell ref="Z23:Z26"/>
+    <mergeCell ref="AA20:AA22"/>
+    <mergeCell ref="AA23:AA29"/>
+    <mergeCell ref="AB23:AB28"/>
+    <mergeCell ref="AC23:AC28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4472,14 +4499,14 @@
       </c>
     </row>
     <row r="4" spans="1:28" ht="21">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
       <c r="G4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="19"/>
@@ -5531,92 +5558,92 @@
       <c r="X20" s="2"/>
     </row>
     <row r="21" spans="1:28" ht="11.25" customHeight="1">
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="31"/>
-      <c r="R21" s="31"/>
-      <c r="S21" s="31"/>
-      <c r="T21" s="31"/>
-      <c r="U21" s="31"/>
-      <c r="V21" s="31"/>
-      <c r="W21" s="31"/>
-      <c r="X21" s="31"/>
-      <c r="Y21" s="31" t="s">
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="33"/>
+      <c r="P21" s="33"/>
+      <c r="Q21" s="33"/>
+      <c r="R21" s="33"/>
+      <c r="S21" s="33"/>
+      <c r="T21" s="33"/>
+      <c r="U21" s="33"/>
+      <c r="V21" s="33"/>
+      <c r="W21" s="33"/>
+      <c r="X21" s="33"/>
+      <c r="Y21" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="Z21" s="31"/>
-      <c r="AA21" s="31" t="s">
+      <c r="Z21" s="33"/>
+      <c r="AA21" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="AB21" s="31" t="s">
+      <c r="AB21" s="33" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="22" spans="1:28">
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="31"/>
-      <c r="R22" s="31"/>
-      <c r="S22" s="31"/>
-      <c r="T22" s="31"/>
-      <c r="U22" s="31"/>
-      <c r="V22" s="31"/>
-      <c r="W22" s="31"/>
-      <c r="X22" s="31"/>
-      <c r="Y22" s="31"/>
-      <c r="Z22" s="31"/>
-      <c r="AA22" s="31"/>
-      <c r="AB22" s="31" t="s">
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="33"/>
+      <c r="R22" s="33"/>
+      <c r="S22" s="33"/>
+      <c r="T22" s="33"/>
+      <c r="U22" s="33"/>
+      <c r="V22" s="33"/>
+      <c r="W22" s="33"/>
+      <c r="X22" s="33"/>
+      <c r="Y22" s="33"/>
+      <c r="Z22" s="33"/>
+      <c r="AA22" s="33"/>
+      <c r="AB22" s="33" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:28">
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="31"/>
-      <c r="Q23" s="31"/>
-      <c r="R23" s="31"/>
-      <c r="S23" s="31"/>
-      <c r="T23" s="31"/>
-      <c r="U23" s="31"/>
-      <c r="V23" s="31"/>
-      <c r="W23" s="31"/>
-      <c r="X23" s="31"/>
-      <c r="Y23" s="31"/>
-      <c r="Z23" s="31"/>
-      <c r="AA23" s="31"/>
-      <c r="AB23" s="31"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="33"/>
+      <c r="Q23" s="33"/>
+      <c r="R23" s="33"/>
+      <c r="S23" s="33"/>
+      <c r="T23" s="33"/>
+      <c r="U23" s="33"/>
+      <c r="V23" s="33"/>
+      <c r="W23" s="33"/>
+      <c r="X23" s="33"/>
+      <c r="Y23" s="33"/>
+      <c r="Z23" s="33"/>
+      <c r="AA23" s="33"/>
+      <c r="AB23" s="33"/>
     </row>
     <row r="24" spans="1:28" ht="11.25" customHeight="1">
       <c r="A24" s="27" t="s">
@@ -5655,13 +5682,13 @@
       <c r="L24" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="M24" s="32" t="s">
+      <c r="M24" s="31" t="s">
         <v>297</v>
       </c>
-      <c r="N24" s="61" t="s">
+      <c r="N24" s="49" t="s">
         <v>291</v>
       </c>
-      <c r="O24" s="52" t="s">
+      <c r="O24" s="53" t="s">
         <v>298</v>
       </c>
       <c r="P24" s="27" t="s">
@@ -5691,16 +5718,16 @@
       <c r="X24" s="27" t="s">
         <v>294</v>
       </c>
-      <c r="Y24" s="55" t="s">
+      <c r="Y24" s="56" t="s">
         <v>295</v>
       </c>
-      <c r="Z24" s="58" t="s">
+      <c r="Z24" s="59" t="s">
         <v>296</v>
       </c>
-      <c r="AA24" s="32" t="s">
+      <c r="AA24" s="31" t="s">
         <v>235</v>
       </c>
-      <c r="AB24" s="49" t="s">
+      <c r="AB24" s="50" t="s">
         <v>302</v>
       </c>
     </row>
@@ -5717,9 +5744,9 @@
       <c r="J25" s="28"/>
       <c r="K25" s="28"/>
       <c r="L25" s="28"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="53"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="54"/>
       <c r="P25" s="28"/>
       <c r="Q25" s="28"/>
       <c r="R25" s="28"/>
@@ -5729,10 +5756,10 @@
       <c r="V25" s="28"/>
       <c r="W25" s="28"/>
       <c r="X25" s="28"/>
-      <c r="Y25" s="56"/>
-      <c r="Z25" s="59"/>
-      <c r="AA25" s="32"/>
-      <c r="AB25" s="50"/>
+      <c r="Y25" s="57"/>
+      <c r="Z25" s="60"/>
+      <c r="AA25" s="31"/>
+      <c r="AB25" s="51"/>
     </row>
     <row r="26" spans="1:28">
       <c r="A26" s="28"/>
@@ -5747,9 +5774,9 @@
       <c r="J26" s="28"/>
       <c r="K26" s="28"/>
       <c r="L26" s="28"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="61"/>
-      <c r="O26" s="53"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="54"/>
       <c r="P26" s="28"/>
       <c r="Q26" s="28"/>
       <c r="R26" s="28"/>
@@ -5759,10 +5786,10 @@
       <c r="V26" s="28"/>
       <c r="W26" s="28"/>
       <c r="X26" s="28"/>
-      <c r="Y26" s="56"/>
-      <c r="Z26" s="59"/>
-      <c r="AA26" s="32"/>
-      <c r="AB26" s="50"/>
+      <c r="Y26" s="57"/>
+      <c r="Z26" s="60"/>
+      <c r="AA26" s="31"/>
+      <c r="AB26" s="51"/>
     </row>
     <row r="27" spans="1:28">
       <c r="A27" s="29"/>
@@ -5777,9 +5804,9 @@
       <c r="J27" s="29"/>
       <c r="K27" s="29"/>
       <c r="L27" s="29"/>
-      <c r="M27" s="32"/>
-      <c r="N27" s="61"/>
-      <c r="O27" s="54"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="49"/>
+      <c r="O27" s="55"/>
       <c r="P27" s="29"/>
       <c r="Q27" s="29"/>
       <c r="R27" s="29"/>
@@ -5789,10 +5816,10 @@
       <c r="V27" s="29"/>
       <c r="W27" s="29"/>
       <c r="X27" s="29"/>
-      <c r="Y27" s="56"/>
-      <c r="Z27" s="59"/>
-      <c r="AA27" s="32"/>
-      <c r="AB27" s="50"/>
+      <c r="Y27" s="57"/>
+      <c r="Z27" s="60"/>
+      <c r="AA27" s="31"/>
+      <c r="AB27" s="51"/>
     </row>
     <row r="28" spans="1:28">
       <c r="E28" s="1"/>
@@ -5800,16 +5827,16 @@
       <c r="K28" s="2"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-      <c r="N28" s="61"/>
+      <c r="N28" s="49"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
       <c r="U28" s="1"/>
       <c r="X28" s="2"/>
-      <c r="Y28" s="56"/>
-      <c r="Z28" s="59"/>
-      <c r="AA28" s="32"/>
-      <c r="AB28" s="50"/>
+      <c r="Y28" s="57"/>
+      <c r="Z28" s="60"/>
+      <c r="AA28" s="31"/>
+      <c r="AB28" s="51"/>
     </row>
     <row r="29" spans="1:28">
       <c r="E29" s="1"/>
@@ -5822,7 +5849,7 @@
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
-      <c r="N29" s="61"/>
+      <c r="N29" s="49"/>
       <c r="R29" s="2"/>
       <c r="S29" s="17" t="s">
         <v>304</v>
@@ -5831,10 +5858,10 @@
         <v>170</v>
       </c>
       <c r="X29" s="2"/>
-      <c r="Y29" s="57"/>
-      <c r="Z29" s="60"/>
-      <c r="AA29" s="32"/>
-      <c r="AB29" s="51"/>
+      <c r="Y29" s="58"/>
+      <c r="Z29" s="61"/>
+      <c r="AA29" s="31"/>
+      <c r="AB29" s="52"/>
     </row>
     <row r="30" spans="1:28" ht="202.5">
       <c r="E30" s="1"/>
@@ -5847,7 +5874,7 @@
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
-      <c r="N30" s="61"/>
+      <c r="N30" s="49"/>
       <c r="R30" s="2"/>
       <c r="S30" s="25" t="s">
         <v>305</v>
@@ -6041,6 +6068,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="AB21:AB23"/>
+    <mergeCell ref="AB24:AB29"/>
+    <mergeCell ref="S24:S27"/>
+    <mergeCell ref="E21:X23"/>
+    <mergeCell ref="V24:V27"/>
+    <mergeCell ref="W24:W27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="O24:O27"/>
+    <mergeCell ref="Y21:Z23"/>
+    <mergeCell ref="Y24:Y29"/>
+    <mergeCell ref="Z24:Z29"/>
+    <mergeCell ref="AA24:AA29"/>
+    <mergeCell ref="AA21:AA23"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
     <mergeCell ref="D24:D27"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="X24:X27"/>
@@ -6057,25 +6103,6 @@
     <mergeCell ref="L24:L27"/>
     <mergeCell ref="R24:R27"/>
     <mergeCell ref="G24:G27"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="AB21:AB23"/>
-    <mergeCell ref="AB24:AB29"/>
-    <mergeCell ref="S24:S27"/>
-    <mergeCell ref="E21:X23"/>
-    <mergeCell ref="V24:V27"/>
-    <mergeCell ref="W24:W27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="O24:O27"/>
-    <mergeCell ref="Y21:Z23"/>
-    <mergeCell ref="Y24:Y29"/>
-    <mergeCell ref="Z24:Z29"/>
-    <mergeCell ref="AA24:AA29"/>
-    <mergeCell ref="AA21:AA23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6085,12 +6112,12 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <tabColor rgb="FFFA7E7E"/>
+    <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A2:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -6411,35 +6438,40 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="33" t="s">
         <v>313</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="G19" s="31" t="s">
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="G19" s="33" t="s">
         <v>314</v>
       </c>
-      <c r="H19" s="31"/>
+      <c r="H19" s="33"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
     </row>
     <row r="22" spans="1:8" ht="11.25" customHeight="1">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="35" t="s">
         <v>174</v>
       </c>
       <c r="B22" s="27" t="s">
@@ -6454,7 +6486,9 @@
       <c r="E22" s="27" t="s">
         <v>310</v>
       </c>
-      <c r="F22" s="27"/>
+      <c r="F22" s="62" t="s">
+        <v>317</v>
+      </c>
       <c r="G22" s="27" t="s">
         <v>311</v>
       </c>
@@ -6463,22 +6497,22 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="46"/>
+      <c r="A23" s="36"/>
       <c r="B23" s="28"/>
       <c r="C23" s="28"/>
       <c r="D23" s="28"/>
       <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
+      <c r="F23" s="63"/>
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="47"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="28"/>
       <c r="C24" s="28"/>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="F24" s="63"/>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
     </row>
@@ -6487,7 +6521,7 @@
       <c r="C25" s="29"/>
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
+      <c r="F25" s="64"/>
       <c r="G25" s="29"/>
       <c r="H25" s="29"/>
     </row>
@@ -6500,13 +6534,21 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="101.25">
+      <c r="F28" s="65" t="s">
+        <v>318</v>
+      </c>
       <c r="G28" s="16"/>
       <c r="H28" s="18" t="s">
         <v>186</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="F19:F21"/>
     <mergeCell ref="H22:H25"/>
     <mergeCell ref="B19:E21"/>
     <mergeCell ref="G19:H21"/>
@@ -6515,10 +6557,6 @@
     <mergeCell ref="D22:D25"/>
     <mergeCell ref="E22:E25"/>
     <mergeCell ref="G22:G25"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>